<commit_message>
poprawki mss11 mss16 mss19 wizc
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/akrg.xlsx
+++ b/Statystyki_2018/Template/akrg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rskowron\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myProjects\prv\statystyki\Statystyki_2018\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{462AE12A-279C-4E22-9DE2-7D8F1FEA0238}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96704B52-900D-44FC-A9A0-7E9893F6B049}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{1A29BF62-F257-4400-9BAA-A806D037713C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{1A29BF62-F257-4400-9BAA-A806D037713C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>Stanowisko</t>
   </si>
@@ -205,6 +205,24 @@
   </si>
   <si>
     <t>ponad 5 lat</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Ua</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>GC merytoryczne</t>
+  </si>
+  <si>
+    <t>Ga merytoryczne</t>
   </si>
 </sst>
 </file>
@@ -501,85 +519,78 @@
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -588,30 +599,37 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -930,261 +948,261 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE3B790-29AE-4BFE-800F-B017217B7895}">
   <dimension ref="A2:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="20"/>
+      <c r="J3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="11" t="s">
+    <row r="4" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
-    </row>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="32"/>
-    </row>
-    <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-    </row>
-    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="32"/>
-    </row>
-    <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-    </row>
-    <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
-    </row>
-    <row r="13" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="32"/>
-    </row>
-    <row r="15" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="32"/>
-    </row>
-    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="32"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1206,195 +1224,224 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251D87B0-394C-433D-91F0-95EB7EA54515}">
-  <dimension ref="A2:AD4"/>
+  <dimension ref="A2:AJ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="35" max="35" width="22.88671875" customWidth="1"/>
+    <col min="36" max="36" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:36" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="12" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="12" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="28" t="s">
+      <c r="V2" s="35"/>
+      <c r="W2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="X2" s="29" t="s">
+      <c r="X2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="Y2" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="16" t="s">
+      <c r="AA2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AH2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16" t="s">
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="17" t="s">
+    <row r="3" spans="1:36" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="2" t="s">
+      <c r="N3" s="20"/>
+      <c r="O3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="21" t="s">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="28"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="8"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="20"/>
       <c r="AA3" s="16"/>
       <c r="AB3" s="16"/>
       <c r="AC3" s="16"/>
       <c r="AD3" s="16"/>
-    </row>
-    <row r="4" spans="1:30" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="11" t="s">
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22"/>
+    </row>
+    <row r="4" spans="1:36" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23" t="s">
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="26" t="s">
+      <c r="T4" s="30"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="27" t="s">
+      <c r="AI4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AD4" s="16"/>
+      <c r="AJ4" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="AB2:AC3"/>
-    <mergeCell ref="AD2:AD4"/>
+  <mergeCells count="36">
+    <mergeCell ref="AH2:AI3"/>
+    <mergeCell ref="AJ2:AJ4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
@@ -1408,11 +1455,17 @@
     <mergeCell ref="T2:T4"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="AE2:AE4"/>
+    <mergeCell ref="AG2:AG4"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W2:W4"/>
     <mergeCell ref="X2:X4"/>
+    <mergeCell ref="AB2:AB4"/>
+    <mergeCell ref="AC2:AC4"/>
+    <mergeCell ref="AD2:AD4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="AF2:AF4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -1422,6 +1475,7 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
+    <mergeCell ref="AA2:AA4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1435,114 +1489,114 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="6" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="36" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="2" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="9"/>
-    </row>
-    <row r="4" spans="1:15" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="11" t="s">
+      <c r="O3" s="37"/>
+    </row>
+    <row r="4" spans="1:15" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="9"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:N2"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:N2"/>
     <mergeCell ref="O2:O4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>

</xml_diff>